<commit_message>
avances en carga controles
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local_web\websites\sivin20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B72A62F-EE5D-4DFE-B015-FC0C795D1D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEABAC0-43E4-4C0D-8171-DC1C73535A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{465527D0-3671-4B53-BEC6-8067D4ED7336}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="2" xr2:uid="{465527D0-3671-4B53-BEC6-8067D4ED7336}"/>
   </bookViews>
   <sheets>
     <sheet name="ninio" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="5" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="6" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="7" r:id="rId3"/>
     <sheet name="etnias" sheetId="3" r:id="rId4"/>
     <sheet name="Resi" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="171">
   <si>
     <t>IdNinio</t>
   </si>
@@ -506,6 +506,51 @@
   </si>
   <si>
     <t xml:space="preserve"> NotVpc</t>
+  </si>
+  <si>
+    <t>$Control['NotId']=$Notifica['NotId'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotFecha']=$Notifica['NotFecha'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotNinio']=$datosNinio['IdNinio'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotUsuario'] = $usuario['id_usuario'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotEfec'] = $Notifica['establecimiento_id'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotMotivo'] = $Notifica['NotMotivo'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotPeso'] = $Notifica['NotPeso'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotTalla'] = $Notifica['NotTalla'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotAo'] = $this-&gt;tablaInsti-&gt;findById($Notifica['establecimiento_id'])['AOP'] ?? '';</t>
+  </si>
+  <si>
+    <t>    $Control['NotEvo'] = $Notifica['NotEvo'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotEtio'] = $Notifica['NotEtio'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotClinica'] = $Notifica['NotClinica'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotObserva'] = ltrim($Notifica['NotObserva']);</t>
+  </si>
+  <si>
+    <t>    $Control['NotObsantro'] = $Notifica['NotObsantro'];</t>
+  </si>
+  <si>
+    <t>    $Control['NotFechaSist'] = new \DateTime();</t>
   </si>
 </sst>
 </file>
@@ -859,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A968B271-23C9-4F25-B970-4325FD966A42}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1145,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958E6D9B-B86E-4DA6-9983-8F6ACD8237C3}">
   <dimension ref="A3:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,130 +1499,141 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D0A363-AE9D-4292-9DEB-E155460ACAA2}">
-  <dimension ref="A1:AK1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFA0E49-5FE4-4020-9C90-8B3C64D115F0}">
+  <dimension ref="A15:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AK1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="89.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L1" t="s">
-        <v>130</v>
-      </c>
-      <c r="M1" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" t="s">
-        <v>132</v>
-      </c>
-      <c r="O1" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>135</v>
-      </c>
-      <c r="R1" t="s">
-        <v>136</v>
-      </c>
-      <c r="S1" t="s">
-        <v>137</v>
-      </c>
-      <c r="T1" t="s">
-        <v>138</v>
-      </c>
-      <c r="U1" t="s">
-        <v>139</v>
-      </c>
-      <c r="V1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W1" t="s">
-        <v>141</v>
-      </c>
-      <c r="X1" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>153</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>155</v>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>